<commit_message>
Major update to code
- output and code folders have been reorganized more efficiently
- focus on analysis 01 (Gridsearch CV) for headline and core inflation for different periods (2019 to 2023)
</commit_message>
<xml_diff>
--- a/output/3_Regression/h19/analysis_01/table_rmse_h19.xlsx
+++ b/output/3_Regression/h19/analysis_01/table_rmse_h19.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0c9b36a04e2b00f1/Documentos/Github/inflation-prediction/output/3_Regression/h19/analysis_01/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_A8B2E42FF830921FD2FE31D2F8F2D3C274D9736E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F707C9B-0049-41BD-B2E8-E2CF8D99301A}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>RW</t>
   </si>
@@ -52,8 +61,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -105,24 +114,394 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="36">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -160,7 +539,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -194,6 +573,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -228,9 +608,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -403,14 +784,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -445,7 +828,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -453,34 +836,34 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>8.496228075794013</v>
+        <v>8.4962280757940132</v>
       </c>
       <c r="D2">
-        <v>0.4520598943774901</v>
+        <v>0.45205989437749011</v>
       </c>
       <c r="E2">
-        <v>0.7641379613477944</v>
+        <v>0.76413796134779444</v>
       </c>
       <c r="F2">
-        <v>0.5347441766660984</v>
+        <v>0.53474417666609841</v>
       </c>
       <c r="G2">
-        <v>0.8186890796079205</v>
+        <v>0.81868907960792048</v>
       </c>
       <c r="H2">
-        <v>0.9558251656047296</v>
+        <v>0.95582516560472963</v>
       </c>
       <c r="I2">
-        <v>0.2926145762776921</v>
+        <v>0.29261457627769211</v>
       </c>
       <c r="J2">
-        <v>0.9067666306148144</v>
+        <v>0.90676663061481444</v>
       </c>
       <c r="K2">
-        <v>3.589568839493083</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>3.5895688394930829</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -491,31 +874,31 @@
         <v>4.907857611397084</v>
       </c>
       <c r="D3">
-        <v>0.7994190807769488</v>
+        <v>0.79941908077694879</v>
       </c>
       <c r="E3">
         <v>1.475041359472093</v>
       </c>
       <c r="F3">
-        <v>0.8460446249119946</v>
+        <v>0.84604462491199461</v>
       </c>
       <c r="G3">
-        <v>0.9473337154936244</v>
+        <v>0.94733371549362444</v>
       </c>
       <c r="H3">
-        <v>0.940809561545269</v>
+        <v>0.94080956154526896</v>
       </c>
       <c r="I3">
         <v>0.7920489118315458</v>
       </c>
       <c r="J3">
-        <v>0.5977225053780251</v>
+        <v>0.59772250537802507</v>
       </c>
       <c r="K3">
-        <v>2.065062247478818</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>2.0650622474788181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -526,31 +909,31 @@
         <v>3.177384523425514</v>
       </c>
       <c r="D4">
-        <v>0.8152365490021812</v>
+        <v>0.81523654900218123</v>
       </c>
       <c r="E4">
         <v>1.636770132311516</v>
       </c>
       <c r="F4">
-        <v>0.8586664879015313</v>
+        <v>0.85866648790153133</v>
       </c>
       <c r="G4">
-        <v>0.8867659831942054</v>
+        <v>0.88676598319420541</v>
       </c>
       <c r="H4">
-        <v>0.800674622339575</v>
+        <v>0.80067462233957498</v>
       </c>
       <c r="I4">
-        <v>0.6627137294121619</v>
+        <v>0.66271372941216189</v>
       </c>
       <c r="J4">
-        <v>0.5330666256665341</v>
+        <v>0.53306662566653407</v>
       </c>
       <c r="K4">
-        <v>1.664896934428114</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+        <v>1.6648969344281139</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -561,31 +944,31 @@
         <v>2.401938569043268</v>
       </c>
       <c r="D5">
-        <v>0.7872224494454658</v>
+        <v>0.78722244944546582</v>
       </c>
       <c r="E5">
-        <v>1.467584502972277</v>
+        <v>1.4675845029722769</v>
       </c>
       <c r="F5">
-        <v>0.8159125396147784</v>
+        <v>0.81591253961477839</v>
       </c>
       <c r="G5">
-        <v>0.8686441144574805</v>
+        <v>0.86864411445748047</v>
       </c>
       <c r="H5">
-        <v>0.7658674592288579</v>
+        <v>0.76586745922885791</v>
       </c>
       <c r="I5">
-        <v>0.6481486296935811</v>
+        <v>0.64814862969358111</v>
       </c>
       <c r="J5">
-        <v>0.7268449826222312</v>
+        <v>0.72684498262223118</v>
       </c>
       <c r="K5">
-        <v>1.581480514263457</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+        <v>1.5814805142634569</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -593,34 +976,34 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1.991561395710716</v>
+        <v>1.9915613957107161</v>
       </c>
       <c r="D6">
-        <v>0.7576708933512192</v>
+        <v>0.75767089335121918</v>
       </c>
       <c r="E6">
-        <v>1.373136569293056</v>
+        <v>1.3731365692930559</v>
       </c>
       <c r="F6">
-        <v>0.7766149174319524</v>
+        <v>0.77661491743195243</v>
       </c>
       <c r="G6">
-        <v>0.8509690409404912</v>
+        <v>0.85096904094049119</v>
       </c>
       <c r="H6">
         <v>0.6709966990244578</v>
       </c>
       <c r="I6">
-        <v>0.6021228207062042</v>
+        <v>0.60212282070620415</v>
       </c>
       <c r="J6">
-        <v>0.6565245070365432</v>
+        <v>0.65652450703654319</v>
       </c>
       <c r="K6">
-        <v>1.631991459584022</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+        <v>1.6319914595840219</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -631,31 +1014,31 @@
         <v>1.695542575542283</v>
       </c>
       <c r="D7">
-        <v>0.7285394580081609</v>
+        <v>0.72853945800816089</v>
       </c>
       <c r="E7">
-        <v>1.191614991704332</v>
+        <v>1.1916149917043319</v>
       </c>
       <c r="F7">
-        <v>0.7425740165044072</v>
+        <v>0.74257401650440724</v>
       </c>
       <c r="G7">
-        <v>0.8272040732212219</v>
+        <v>0.82720407322122191</v>
       </c>
       <c r="H7">
-        <v>0.6548184632085891</v>
+        <v>0.65481846320858905</v>
       </c>
       <c r="I7">
-        <v>0.7004958900693986</v>
+        <v>0.70049589006939861</v>
       </c>
       <c r="J7">
-        <v>0.6200095965515262</v>
+        <v>0.62000959655152621</v>
       </c>
       <c r="K7">
-        <v>1.698395358084272</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+        <v>1.6983953580842721</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -663,25 +1046,25 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.490358219395635</v>
+        <v>1.4903582193956351</v>
       </c>
       <c r="D8">
-        <v>0.70734020020634</v>
+        <v>0.70734020020634003</v>
       </c>
       <c r="E8">
-        <v>1.051207741149284</v>
+        <v>1.0512077411492839</v>
       </c>
       <c r="F8">
-        <v>0.7180443815806271</v>
+        <v>0.71804438158062711</v>
       </c>
       <c r="G8">
         <v>0.8117910477018605</v>
       </c>
       <c r="H8">
-        <v>0.7847567293251673</v>
+        <v>0.78475672932516727</v>
       </c>
       <c r="I8">
-        <v>0.681266936905257</v>
+        <v>0.68126693690525697</v>
       </c>
       <c r="J8">
         <v>0.5679128012497856</v>
@@ -690,7 +1073,7 @@
         <v>1.703093263588958</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -701,31 +1084,31 @@
         <v>1.34974051782543</v>
       </c>
       <c r="D9">
-        <v>0.6898448208667882</v>
+        <v>0.68984482086678822</v>
       </c>
       <c r="E9">
-        <v>0.9551311838257283</v>
+        <v>0.95513118382572826</v>
       </c>
       <c r="F9">
-        <v>0.6986229331126608</v>
+        <v>0.69862293311266077</v>
       </c>
       <c r="G9">
-        <v>0.7979983205282568</v>
+        <v>0.79799832052825681</v>
       </c>
       <c r="H9">
-        <v>0.7678283517498889</v>
+        <v>0.76782835174988895</v>
       </c>
       <c r="I9">
-        <v>0.6281764351403066</v>
+        <v>0.62817643514030663</v>
       </c>
       <c r="J9">
-        <v>0.5218895408829199</v>
+        <v>0.52188954088291994</v>
       </c>
       <c r="K9">
-        <v>1.667065603115281</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+        <v>1.6670656031152811</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -733,34 +1116,34 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1.263237163434518</v>
+        <v>1.2632371634345181</v>
       </c>
       <c r="D10">
-        <v>0.6740653757912209</v>
+        <v>0.67406537579122094</v>
       </c>
       <c r="E10">
-        <v>0.8814639690998075</v>
+        <v>0.88146396909980751</v>
       </c>
       <c r="F10">
-        <v>0.6823626876155212</v>
+        <v>0.68236268761552121</v>
       </c>
       <c r="G10">
-        <v>0.7825619606306912</v>
+        <v>0.78256196063069117</v>
       </c>
       <c r="H10">
-        <v>0.7084183097465018</v>
+        <v>0.70841830974650177</v>
       </c>
       <c r="I10">
-        <v>0.6097567301020351</v>
+        <v>0.60975673010203513</v>
       </c>
       <c r="J10">
-        <v>0.4824413007900843</v>
+        <v>0.48244130079008429</v>
       </c>
       <c r="K10">
         <v>1.61481400233965</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -771,31 +1154,31 @@
         <v>1.22070579880344</v>
       </c>
       <c r="D11">
-        <v>0.6583786247172502</v>
+        <v>0.65837862471725017</v>
       </c>
       <c r="E11">
         <v>0.816628110745522</v>
       </c>
       <c r="F11">
-        <v>0.6657995911223448</v>
+        <v>0.66579959112234477</v>
       </c>
       <c r="G11">
-        <v>0.7683645635180744</v>
+        <v>0.76836456351807436</v>
       </c>
       <c r="H11">
-        <v>0.7143967228032101</v>
+        <v>0.71439672280321009</v>
       </c>
       <c r="I11">
-        <v>0.585259018926796</v>
+        <v>0.58525901892679599</v>
       </c>
       <c r="J11">
-        <v>0.4470218499740267</v>
+        <v>0.44702184997402672</v>
       </c>
       <c r="K11">
-        <v>1.549598847359212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+        <v>1.5495988473592119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -806,31 +1189,31 @@
         <v>1.238977160178699</v>
       </c>
       <c r="D12">
-        <v>0.6462548050059576</v>
+        <v>0.64625480500595756</v>
       </c>
       <c r="E12">
-        <v>0.786627841905656</v>
+        <v>0.78662784190565604</v>
       </c>
       <c r="F12">
-        <v>0.6534463448444208</v>
+        <v>0.65344634484442077</v>
       </c>
       <c r="G12">
-        <v>0.7547185479834574</v>
+        <v>0.75471854798345739</v>
       </c>
       <c r="H12">
-        <v>0.7622652840281687</v>
+        <v>0.76226528402816873</v>
       </c>
       <c r="I12">
-        <v>0.5478285030626304</v>
+        <v>0.54782850306263042</v>
       </c>
       <c r="J12">
-        <v>0.416137913239203</v>
+        <v>0.41613791323920302</v>
       </c>
       <c r="K12">
         <v>1.499352559496804</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -841,31 +1224,1417 @@
         <v>1.332218677211602</v>
       </c>
       <c r="D13">
-        <v>0.6333690361458508</v>
+        <v>0.63336903614585083</v>
       </c>
       <c r="E13">
-        <v>0.7320925911685454</v>
+        <v>0.73209259116854541</v>
       </c>
       <c r="F13">
-        <v>0.639689966829154</v>
+        <v>0.63968996682915402</v>
       </c>
       <c r="G13">
-        <v>0.7407888123700428</v>
+        <v>0.74078881237004279</v>
       </c>
       <c r="H13">
-        <v>0.7129388403246725</v>
+        <v>0.71293884032467247</v>
       </c>
       <c r="I13">
-        <v>0.5167254727385854</v>
+        <v>0.51672547273858538</v>
       </c>
       <c r="J13">
-        <v>0.3998806190697239</v>
+        <v>0.39988061906972389</v>
       </c>
       <c r="K13">
-        <v>1.447491414246182</v>
+        <v>1.4474914142461821</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{174232F6-91F5-4C74-AB68-42CBBAE21842}">
+  <dimension ref="A9:M19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="13" width="7.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2</v>
+      </c>
+      <c r="D9" s="1">
+        <v>3</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>7</v>
+      </c>
+      <c r="I9" s="1">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1">
+        <v>9</v>
+      </c>
+      <c r="K9" s="1">
+        <v>10</v>
+      </c>
+      <c r="L9" s="1">
+        <v>11</v>
+      </c>
+      <c r="M9" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="2">
+        <v>8.4962280757940132</v>
+      </c>
+      <c r="C11" s="2">
+        <v>4.907857611397084</v>
+      </c>
+      <c r="D11" s="2">
+        <v>3.177384523425514</v>
+      </c>
+      <c r="E11" s="2">
+        <v>2.401938569043268</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1.9915613957107161</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1.695542575542283</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1.4903582193956351</v>
+      </c>
+      <c r="I11" s="2">
+        <v>1.34974051782543</v>
+      </c>
+      <c r="J11" s="2">
+        <v>1.2632371634345181</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.22070579880344</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1.238977160178699</v>
+      </c>
+      <c r="M11" s="2">
+        <v>1.332218677211602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.45205989437749011</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.79941908077694879</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.81523654900218123</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.78722244944546582</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.75767089335121918</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.72853945800816089</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.70734020020634003</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.68984482086678822</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.67406537579122094</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.65837862471725017</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.64625480500595756</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.63336903614585083</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.76413796134779444</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.475041359472093</v>
+      </c>
+      <c r="D13" s="2">
+        <v>1.636770132311516</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.4675845029722769</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1.3731365692930559</v>
+      </c>
+      <c r="G13" s="2">
+        <v>1.1916149917043319</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1.0512077411492839</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.95513118382572826</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.88146396909980751</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.816628110745522</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.78662784190565604</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.73209259116854541</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.53474417666609841</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.84604462491199461</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.85866648790153133</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.81591253961477839</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.77661491743195243</v>
+      </c>
+      <c r="G14" s="2">
+        <v>0.74257401650440724</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.71804438158062711</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.69862293311266077</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.68236268761552121</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.66579959112234477</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.65344634484442077</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.63968996682915402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.81868907960792048</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.94733371549362444</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.88676598319420541</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.86864411445748047</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.85096904094049119</v>
+      </c>
+      <c r="G15" s="2">
+        <v>0.82720407322122191</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.8117910477018605</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.79799832052825681</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.78256196063069117</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.76836456351807436</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.75471854798345739</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.74078881237004279</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.95582516560472963</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.94080956154526896</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.80067462233957498</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.76586745922885791</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.6709966990244578</v>
+      </c>
+      <c r="G16" s="2">
+        <v>0.65481846320858905</v>
+      </c>
+      <c r="H16" s="2">
+        <v>0.78475672932516727</v>
+      </c>
+      <c r="I16" s="2">
+        <v>0.76782835174988895</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.70841830974650177</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.71439672280321009</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.76226528402816873</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.71293884032467247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.29261457627769211</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.7920489118315458</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.66271372941216189</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.64814862969358111</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.60212282070620415</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.70049589006939861</v>
+      </c>
+      <c r="H17" s="2">
+        <v>0.68126693690525697</v>
+      </c>
+      <c r="I17" s="2">
+        <v>0.62817643514030663</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.60975673010203513</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.58525901892679599</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.54782850306263042</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.51672547273858538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.90676663061481444</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.59772250537802507</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.53306662566653407</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.72684498262223118</v>
+      </c>
+      <c r="F18" s="2">
+        <v>0.65652450703654319</v>
+      </c>
+      <c r="G18" s="2">
+        <v>0.62000959655152621</v>
+      </c>
+      <c r="H18" s="2">
+        <v>0.5679128012497856</v>
+      </c>
+      <c r="I18" s="2">
+        <v>0.52188954088291994</v>
+      </c>
+      <c r="J18" s="2">
+        <v>0.48244130079008429</v>
+      </c>
+      <c r="K18" s="2">
+        <v>0.44702184997402672</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.41613791323920302</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.39988061906972389</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="2">
+        <v>3.5895688394930829</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2.0650622474788181</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1.6648969344281139</v>
+      </c>
+      <c r="E19" s="2">
+        <v>1.5814805142634569</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1.6319914595840219</v>
+      </c>
+      <c r="G19" s="2">
+        <v>1.6983953580842721</v>
+      </c>
+      <c r="H19" s="2">
+        <v>1.703093263588958</v>
+      </c>
+      <c r="I19" s="2">
+        <v>1.6670656031152811</v>
+      </c>
+      <c r="J19" s="2">
+        <v>1.61481400233965</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1.5495988473592119</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1.499352559496804</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1.4474914142461821</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M10:M19">
+    <cfRule type="top10" dxfId="35" priority="12" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L10:L19">
+    <cfRule type="top10" dxfId="34" priority="11" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K10:K19">
+    <cfRule type="top10" dxfId="33" priority="10" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10:J19">
+    <cfRule type="top10" dxfId="32" priority="9" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I10:I19">
+    <cfRule type="top10" dxfId="31" priority="8" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:H19">
+    <cfRule type="top10" dxfId="30" priority="7" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G10:G19">
+    <cfRule type="top10" dxfId="29" priority="6" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10:F19">
+    <cfRule type="top10" dxfId="28" priority="5" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10:E19">
+    <cfRule type="top10" dxfId="27" priority="4" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10:D19">
+    <cfRule type="top10" dxfId="26" priority="3" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:C19">
+    <cfRule type="top10" dxfId="25" priority="2" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:B19">
+    <cfRule type="top10" dxfId="24" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C5DF46-340B-49B0-A765-E88EB070CF91}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.4962280757940132</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.907857611397084</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.177384523425514</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.401938569043268</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.9915613957107161</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.695542575542283</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.4903582193956351</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.34974051782543</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.2632371634345181</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.22070579880344</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.238977160178699</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1.332218677211602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.45205989437749011</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.79941908077694879</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.81523654900218123</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.78722244944546582</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.75767089335121918</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.72853945800816089</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.70734020020634003</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.68984482086678822</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.67406537579122094</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.65837862471725017</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.64625480500595756</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.63336903614585083</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.76413796134779444</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.475041359472093</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.636770132311516</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.4675845029722769</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.3731365692930559</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.1916149917043319</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.0512077411492839</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.95513118382572826</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.88146396909980751</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.816628110745522</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.78662784190565604</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.73209259116854541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.53474417666609841</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.84604462491199461</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.85866648790153133</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.81591253961477839</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.77661491743195243</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.74257401650440724</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.71804438158062711</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.69862293311266077</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.68236268761552121</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.66579959112234477</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.65344634484442077</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.63968996682915402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.81868907960792048</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.94733371549362444</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.88676598319420541</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.86864411445748047</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.85096904094049119</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.82720407322122191</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.8117910477018605</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.79799832052825681</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.78256196063069117</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.76836456351807436</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.75471854798345739</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.74078881237004279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.95582516560472963</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.94080956154526896</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.80067462233957498</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.76586745922885791</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.6709966990244578</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.65481846320858905</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.78475672932516727</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.76782835174988895</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.70841830974650177</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.71439672280321009</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.76226528402816873</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.71293884032467247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.29261457627769211</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.7920489118315458</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.66271372941216189</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.64814862969358111</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.60212282070620415</v>
+      </c>
+      <c r="G9" s="2">
+        <v>0.70049589006939861</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0.68126693690525697</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0.62817643514030663</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.60975673010203513</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.58525901892679599</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.54782850306263042</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.51672547273858538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>3.5895688394930829</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2.0650622474788181</v>
+      </c>
+      <c r="D10" s="2">
+        <v>1.6648969344281139</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.5814805142634569</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1.6319914595840219</v>
+      </c>
+      <c r="G10" s="2">
+        <v>1.6983953580842721</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1.703093263588958</v>
+      </c>
+      <c r="I10" s="2">
+        <v>1.6670656031152811</v>
+      </c>
+      <c r="J10" s="2">
+        <v>1.61481400233965</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1.5495988473592119</v>
+      </c>
+      <c r="L10" s="2">
+        <v>1.499352559496804</v>
+      </c>
+      <c r="M10" s="2">
+        <v>1.4474914142461821</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M2:M10">
+    <cfRule type="top10" dxfId="23" priority="13" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L10">
+    <cfRule type="top10" dxfId="22" priority="15" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K10">
+    <cfRule type="top10" dxfId="21" priority="17" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J10">
+    <cfRule type="top10" dxfId="20" priority="19" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I10">
+    <cfRule type="top10" dxfId="19" priority="21" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H10">
+    <cfRule type="top10" dxfId="18" priority="23" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G10">
+    <cfRule type="top10" dxfId="17" priority="25" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F10">
+    <cfRule type="top10" dxfId="16" priority="27" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E10">
+    <cfRule type="top10" dxfId="15" priority="29" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D10">
+    <cfRule type="top10" dxfId="14" priority="31" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C10">
+    <cfRule type="top10" dxfId="13" priority="33" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B10">
+    <cfRule type="top10" dxfId="12" priority="35" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0BF137-4A38-4CFC-95C2-B7FE3455E22A}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2">
+        <v>8.4962280757940132</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4.907857611397084</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.177384523425514</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2.401938569043268</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1.9915613957107161</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1.695542575542283</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1.4903582193956351</v>
+      </c>
+      <c r="I3" s="2">
+        <v>1.34974051782543</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.2632371634345181</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.22070579880344</v>
+      </c>
+      <c r="L3" s="2">
+        <v>1.238977160178699</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1.332218677211602</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.45205989437749011</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.79941908077694879</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.81523654900218123</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.78722244944546582</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.75767089335121918</v>
+      </c>
+      <c r="G4" s="2">
+        <v>0.72853945800816089</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0.70734020020634003</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0.68984482086678822</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.67406537579122094</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.65837862471725017</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.64625480500595756</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.63336903614585083</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.76413796134779444</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.475041359472093</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.636770132311516</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.4675845029722769</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.3731365692930559</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.1916149917043319</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1.0512077411492839</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.95513118382572826</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.88146396909980751</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.816628110745522</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.78662784190565604</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.73209259116854541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.53474417666609841</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.84604462491199461</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.85866648790153133</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.81591253961477839</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.77661491743195243</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0.74257401650440724</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0.71804438158062711</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0.69862293311266077</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.68236268761552121</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.66579959112234477</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.65344634484442077</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.63968996682915402</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.81868907960792048</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.94733371549362444</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.88676598319420541</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.86864411445748047</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.85096904094049119</v>
+      </c>
+      <c r="G7" s="2">
+        <v>0.82720407322122191</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0.8117910477018605</v>
+      </c>
+      <c r="I7" s="2">
+        <v>0.79799832052825681</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.78256196063069117</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.76836456351807436</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.75471854798345739</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.74078881237004279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.95582516560472963</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.94080956154526896</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.80067462233957498</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.76586745922885791</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0.6709966990244578</v>
+      </c>
+      <c r="G8" s="2">
+        <v>0.65481846320858905</v>
+      </c>
+      <c r="H8" s="2">
+        <v>0.78475672932516727</v>
+      </c>
+      <c r="I8" s="2">
+        <v>0.76782835174988895</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.70841830974650177</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.71439672280321009</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.76226528402816873</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.71293884032467247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3.5895688394930829</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.0650622474788181</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.6648969344281139</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.5814805142634569</v>
+      </c>
+      <c r="F9" s="2">
+        <v>1.6319914595840219</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1.6983953580842721</v>
+      </c>
+      <c r="H9" s="2">
+        <v>1.703093263588958</v>
+      </c>
+      <c r="I9" s="2">
+        <v>1.6670656031152811</v>
+      </c>
+      <c r="J9" s="2">
+        <v>1.61481400233965</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.5495988473592119</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1.499352559496804</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1.4474914142461821</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="M2:M9">
+    <cfRule type="top10" dxfId="11" priority="36" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L9">
+    <cfRule type="top10" dxfId="10" priority="38" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K9">
+    <cfRule type="top10" dxfId="9" priority="40" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J9">
+    <cfRule type="top10" dxfId="8" priority="42" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I9">
+    <cfRule type="top10" dxfId="7" priority="44" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H9">
+    <cfRule type="top10" dxfId="6" priority="46" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G9">
+    <cfRule type="top10" dxfId="5" priority="48" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F9">
+    <cfRule type="top10" dxfId="4" priority="50" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E9">
+    <cfRule type="top10" dxfId="3" priority="52" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D9">
+    <cfRule type="top10" dxfId="2" priority="54" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C9">
+    <cfRule type="top10" dxfId="1" priority="56" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B9">
+    <cfRule type="top10" dxfId="0" priority="58" bottom="1" rank="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>